<commit_message>
super summary table feature complete
</commit_message>
<xml_diff>
--- a/data/biolog_results/Metabolites Listing.xlsx
+++ b/data/biolog_results/Metabolites Listing.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Biomedicine\lmurinus_gem\data\biolog_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E54811-D410-4687-AA8C-AEF4D7428C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1528E92-9AF6-44B4-9EE4-88F746FECB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14205" yWindow="0" windowWidth="14595" windowHeight="17280" xr2:uid="{CF095307-2C1C-4547-AA63-7BB7228FFDBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{CF095307-2C1C-4547-AA63-7BB7228FFDBF}"/>
   </bookViews>
   <sheets>
     <sheet name="BIOLOG" sheetId="1" r:id="rId1"/>
+    <sheet name="KWOJI" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="504">
   <si>
     <t>Plate Pos.</t>
   </si>
@@ -1176,6 +1177,378 @@
   </si>
   <si>
     <t>C9H11N2O8P</t>
+  </si>
+  <si>
+    <t>cpd00009_e0</t>
+  </si>
+  <si>
+    <t>cpd00205_e0</t>
+  </si>
+  <si>
+    <t>cpd00067_e0</t>
+  </si>
+  <si>
+    <t>cpd00254_e0</t>
+  </si>
+  <si>
+    <t>cpd00048_e0</t>
+  </si>
+  <si>
+    <t>cpd00001_e0</t>
+  </si>
+  <si>
+    <t>cpd00030_e0</t>
+  </si>
+  <si>
+    <t>cpd00013_e0</t>
+  </si>
+  <si>
+    <t>cpd00099_e0</t>
+  </si>
+  <si>
+    <t>cpd10515_e0</t>
+  </si>
+  <si>
+    <t>cpd00971_e0</t>
+  </si>
+  <si>
+    <t>cpd00011_e0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cpd00149_e0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cpd00063_e0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cpd00034_e0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cpd00058_e0 </t>
+  </si>
+  <si>
+    <t>cpd00029_e0</t>
+  </si>
+  <si>
+    <t>cpd00028_e0</t>
+  </si>
+  <si>
+    <t>cpd00322_e0</t>
+  </si>
+  <si>
+    <t>cpd00060_e0</t>
+  </si>
+  <si>
+    <t>cpd00066_e0</t>
+  </si>
+  <si>
+    <t>cpd00119_e0</t>
+  </si>
+  <si>
+    <t>cpd00053_e0</t>
+  </si>
+  <si>
+    <t>cpd00023_e0</t>
+  </si>
+  <si>
+    <t>cpd00132_e0</t>
+  </si>
+  <si>
+    <t>cpd00041_e0</t>
+  </si>
+  <si>
+    <t>cpd00069_e0</t>
+  </si>
+  <si>
+    <t>cpd00065_e0</t>
+  </si>
+  <si>
+    <t>cpd00035_e0</t>
+  </si>
+  <si>
+    <t>cpd00156_e0</t>
+  </si>
+  <si>
+    <t>cpd00051_e0</t>
+  </si>
+  <si>
+    <t>cpd00129_e0</t>
+  </si>
+  <si>
+    <t>cpd00033_e0</t>
+  </si>
+  <si>
+    <t>cpd00039_e0</t>
+  </si>
+  <si>
+    <t>cpd00161_e0</t>
+  </si>
+  <si>
+    <t>cpd00107_e0</t>
+  </si>
+  <si>
+    <t>cpd00054_e0</t>
+  </si>
+  <si>
+    <t>cpd00084_e0</t>
+  </si>
+  <si>
+    <t>cpd00311_e0</t>
+  </si>
+  <si>
+    <t>cpd00182_e0</t>
+  </si>
+  <si>
+    <t>cpd01217_e0</t>
+  </si>
+  <si>
+    <t>cpd00184_e0</t>
+  </si>
+  <si>
+    <t>cpd00092_e0</t>
+  </si>
+  <si>
+    <t>cpd00218_e0</t>
+  </si>
+  <si>
+    <t>cpd00305_e0</t>
+  </si>
+  <si>
+    <t>cpd00644_e0</t>
+  </si>
+  <si>
+    <t>cpd00220_e0</t>
+  </si>
+  <si>
+    <t>cpd00393_e0</t>
+  </si>
+  <si>
+    <t>cpd00104_e0</t>
+  </si>
+  <si>
+    <t>cpd11606_e0</t>
+  </si>
+  <si>
+    <t>Phosphate</t>
+  </si>
+  <si>
+    <t>K+</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>HO4P</t>
+  </si>
+  <si>
+    <t>H+</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Mg</t>
+  </si>
+  <si>
+    <t>Sulfate</t>
+  </si>
+  <si>
+    <t>O4S</t>
+  </si>
+  <si>
+    <t>Mn2+</t>
+  </si>
+  <si>
+    <t>Mn</t>
+  </si>
+  <si>
+    <t>NH3</t>
+  </si>
+  <si>
+    <t>H4N</t>
+  </si>
+  <si>
+    <t>Cl-</t>
+  </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>Fe+2</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>Na+</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>Co2+</t>
+  </si>
+  <si>
+    <t>Co</t>
+  </si>
+  <si>
+    <t>Ca2+</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>Zn2+</t>
+  </si>
+  <si>
+    <t>Zn</t>
+  </si>
+  <si>
+    <t>Cu2+</t>
+  </si>
+  <si>
+    <t>Cu</t>
+  </si>
+  <si>
+    <t>Acetate</t>
+  </si>
+  <si>
+    <t>Heme</t>
+  </si>
+  <si>
+    <t>C34H30FeN4O4</t>
+  </si>
+  <si>
+    <t>L-Isoleucine</t>
+  </si>
+  <si>
+    <t>C6H13NO2</t>
+  </si>
+  <si>
+    <t>L-Histidine</t>
+  </si>
+  <si>
+    <t>C6H9N3O2</t>
+  </si>
+  <si>
+    <t>L-Glutamate</t>
+  </si>
+  <si>
+    <t>L-Aspartate</t>
+  </si>
+  <si>
+    <t>L-Tyrosine</t>
+  </si>
+  <si>
+    <t>C9H11NO3</t>
+  </si>
+  <si>
+    <t>L-Tryptophan</t>
+  </si>
+  <si>
+    <t>C11H12N2O2</t>
+  </si>
+  <si>
+    <t>L-Arginine</t>
+  </si>
+  <si>
+    <t>C6H15N4O2</t>
+  </si>
+  <si>
+    <t>L-Proline</t>
+  </si>
+  <si>
+    <t>C5H9NO2</t>
+  </si>
+  <si>
+    <t>Glycine</t>
+  </si>
+  <si>
+    <t>C2H5NO2</t>
+  </si>
+  <si>
+    <t>L-Lysine</t>
+  </si>
+  <si>
+    <t>C6H15N2O2</t>
+  </si>
+  <si>
+    <t>L-Leucine</t>
+  </si>
+  <si>
+    <t>L-Cysteine</t>
+  </si>
+  <si>
+    <t>C3H7NO2S</t>
+  </si>
+  <si>
+    <t>Guanosine</t>
+  </si>
+  <si>
+    <t>C10H13N5O5</t>
+  </si>
+  <si>
+    <t>Adenosine</t>
+  </si>
+  <si>
+    <t>C10H13N5O4</t>
+  </si>
+  <si>
+    <t>Xanthosine</t>
+  </si>
+  <si>
+    <t>C10H12N4O6</t>
+  </si>
+  <si>
+    <t>Uracil</t>
+  </si>
+  <si>
+    <t>C4H4N2O2</t>
+  </si>
+  <si>
+    <t>Niacin</t>
+  </si>
+  <si>
+    <t>C6H4NO2</t>
+  </si>
+  <si>
+    <t>Thiamin</t>
+  </si>
+  <si>
+    <t>C12H17N4OS</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>C9H16NO5</t>
+  </si>
+  <si>
+    <t>Riboflavin</t>
+  </si>
+  <si>
+    <t>C17H19N4O6</t>
+  </si>
+  <si>
+    <t>Folate</t>
+  </si>
+  <si>
+    <t>C19H17N7O6</t>
+  </si>
+  <si>
+    <t>BIOT</t>
+  </si>
+  <si>
+    <t>C10H15N2O3S</t>
+  </si>
+  <si>
+    <t>Menaquinone 7</t>
+  </si>
+  <si>
+    <t>C46H64O2</t>
   </si>
 </sst>
 </file>
@@ -1220,7 +1593,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9E1F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1552,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEA9BD9-40AF-47D8-BDE5-5EF927DAAE93}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2989,4 +3384,587 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6742B5D-D9C6-40F6-956B-8D4672EB2283}">
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>431</v>
+      </c>
+      <c r="B3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>434</v>
+      </c>
+      <c r="B4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C4" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>436</v>
+      </c>
+      <c r="B5" t="s">
+        <v>383</v>
+      </c>
+      <c r="C5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>437</v>
+      </c>
+      <c r="B6" t="s">
+        <v>384</v>
+      </c>
+      <c r="C6" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" t="s">
+        <v>385</v>
+      </c>
+      <c r="C7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B8" t="s">
+        <v>386</v>
+      </c>
+      <c r="C8" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>441</v>
+      </c>
+      <c r="B9" t="s">
+        <v>387</v>
+      </c>
+      <c r="C9" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>443</v>
+      </c>
+      <c r="B10" t="s">
+        <v>388</v>
+      </c>
+      <c r="C10" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>445</v>
+      </c>
+      <c r="B11" t="s">
+        <v>389</v>
+      </c>
+      <c r="C11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>447</v>
+      </c>
+      <c r="B12" t="s">
+        <v>390</v>
+      </c>
+      <c r="C12" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>449</v>
+      </c>
+      <c r="B13" t="s">
+        <v>391</v>
+      </c>
+      <c r="C13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>450</v>
+      </c>
+      <c r="B14" t="s">
+        <v>392</v>
+      </c>
+      <c r="C14" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>452</v>
+      </c>
+      <c r="B15" t="s">
+        <v>393</v>
+      </c>
+      <c r="C15" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>454</v>
+      </c>
+      <c r="B16" t="s">
+        <v>394</v>
+      </c>
+      <c r="C16" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>456</v>
+      </c>
+      <c r="B17" t="s">
+        <v>395</v>
+      </c>
+      <c r="C17" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>458</v>
+      </c>
+      <c r="B18" t="s">
+        <v>396</v>
+      </c>
+      <c r="C18" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>459</v>
+      </c>
+      <c r="B19" t="s">
+        <v>397</v>
+      </c>
+      <c r="C19" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>461</v>
+      </c>
+      <c r="B20" t="s">
+        <v>398</v>
+      </c>
+      <c r="C20" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" t="s">
+        <v>399</v>
+      </c>
+      <c r="C21" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" t="s">
+        <v>400</v>
+      </c>
+      <c r="C22" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>463</v>
+      </c>
+      <c r="B23" t="s">
+        <v>401</v>
+      </c>
+      <c r="C23" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" t="s">
+        <v>402</v>
+      </c>
+      <c r="C24" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>465</v>
+      </c>
+      <c r="B25" t="s">
+        <v>403</v>
+      </c>
+      <c r="C25" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" t="s">
+        <v>404</v>
+      </c>
+      <c r="C26" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>466</v>
+      </c>
+      <c r="B27" t="s">
+        <v>405</v>
+      </c>
+      <c r="C27" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>467</v>
+      </c>
+      <c r="B28" t="s">
+        <v>406</v>
+      </c>
+      <c r="C28" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>469</v>
+      </c>
+      <c r="B29" t="s">
+        <v>407</v>
+      </c>
+      <c r="C29" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" t="s">
+        <v>408</v>
+      </c>
+      <c r="C30" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31" t="s">
+        <v>409</v>
+      </c>
+      <c r="C31" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>471</v>
+      </c>
+      <c r="B32" t="s">
+        <v>410</v>
+      </c>
+      <c r="C32" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>473</v>
+      </c>
+      <c r="B33" t="s">
+        <v>411</v>
+      </c>
+      <c r="C33" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>475</v>
+      </c>
+      <c r="B34" t="s">
+        <v>412</v>
+      </c>
+      <c r="C34" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>477</v>
+      </c>
+      <c r="B35" t="s">
+        <v>413</v>
+      </c>
+      <c r="C35" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>180</v>
+      </c>
+      <c r="B36" t="s">
+        <v>414</v>
+      </c>
+      <c r="C36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>479</v>
+      </c>
+      <c r="B37" t="s">
+        <v>415</v>
+      </c>
+      <c r="C37" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>178</v>
+      </c>
+      <c r="B38" t="s">
+        <v>416</v>
+      </c>
+      <c r="C38" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>480</v>
+      </c>
+      <c r="B39" t="s">
+        <v>417</v>
+      </c>
+      <c r="C39" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>482</v>
+      </c>
+      <c r="B40" t="s">
+        <v>418</v>
+      </c>
+      <c r="C40" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>484</v>
+      </c>
+      <c r="B41" t="s">
+        <v>419</v>
+      </c>
+      <c r="C41" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>486</v>
+      </c>
+      <c r="B42" t="s">
+        <v>420</v>
+      </c>
+      <c r="C42" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>421</v>
+      </c>
+      <c r="C43" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>488</v>
+      </c>
+      <c r="B44" t="s">
+        <v>422</v>
+      </c>
+      <c r="C44" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>490</v>
+      </c>
+      <c r="B45" t="s">
+        <v>423</v>
+      </c>
+      <c r="C45" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>492</v>
+      </c>
+      <c r="B46" t="s">
+        <v>424</v>
+      </c>
+      <c r="C46" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>494</v>
+      </c>
+      <c r="B47" t="s">
+        <v>425</v>
+      </c>
+      <c r="C47" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>496</v>
+      </c>
+      <c r="B48" t="s">
+        <v>426</v>
+      </c>
+      <c r="C48" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>498</v>
+      </c>
+      <c r="B49" t="s">
+        <v>427</v>
+      </c>
+      <c r="C49" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>500</v>
+      </c>
+      <c r="B50" t="s">
+        <v>428</v>
+      </c>
+      <c r="C50" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>502</v>
+      </c>
+      <c r="B51" t="s">
+        <v>429</v>
+      </c>
+      <c r="C51" t="s">
+        <v>503</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Preparing for package overhaul
</commit_message>
<xml_diff>
--- a/data/biolog_results/Metabolites Listing.xlsx
+++ b/data/biolog_results/Metabolites Listing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Biomedicine\lmurinus_gem\data\biolog_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1528E92-9AF6-44B4-9EE4-88F746FECB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902F30AC-0A58-4FB9-AB97-C1EBFC25C128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{CF095307-2C1C-4547-AA63-7BB7228FFDBF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{CF095307-2C1C-4547-AA63-7BB7228FFDBF}"/>
   </bookViews>
   <sheets>
     <sheet name="BIOLOG" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="510">
   <si>
     <t>Plate Pos.</t>
   </si>
@@ -1549,6 +1549,24 @@
   </si>
   <si>
     <t>C46H64O2</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Miscellaneous / Other</t>
+  </si>
+  <si>
+    <t>Carbohydrates &amp; Derivatives</t>
+  </si>
+  <si>
+    <t>Organic Acids &amp; Derivatives</t>
+  </si>
+  <si>
+    <t>Amino Acids &amp; Peptides</t>
+  </si>
+  <si>
+    <t>Nucleosides &amp; Nucleotides</t>
   </si>
 </sst>
 </file>
@@ -1584,38 +1602,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9E1F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1945,10 +1949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEA9BD9-40AF-47D8-BDE5-5EF927DAAE93}">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J93" sqref="J93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,9 +1962,10 @@
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1976,8 +1981,11 @@
       <c r="E1" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1990,8 +1998,11 @@
       <c r="D2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2004,8 +2015,11 @@
       <c r="D3" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="3" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -2018,8 +2032,11 @@
       <c r="D4" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="3" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -2032,8 +2049,11 @@
       <c r="D5" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="3" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -2049,8 +2069,11 @@
       <c r="E6" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="4" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -2063,8 +2086,11 @@
       <c r="D7" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="5" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -2077,8 +2103,11 @@
       <c r="D8" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -2091,8 +2120,11 @@
       <c r="D9" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -2105,8 +2137,11 @@
       <c r="D10" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -2119,8 +2154,11 @@
       <c r="D11" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -2136,8 +2174,11 @@
       <c r="E12" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -2150,8 +2191,11 @@
       <c r="D13" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -2164,8 +2208,11 @@
       <c r="D14" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -2181,8 +2228,11 @@
       <c r="E15" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -2195,8 +2245,11 @@
       <c r="D16" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -2209,8 +2262,11 @@
       <c r="D17" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
@@ -2223,8 +2279,11 @@
       <c r="D18" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
@@ -2237,8 +2296,11 @@
       <c r="D19" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -2251,8 +2313,11 @@
       <c r="D20" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -2268,8 +2333,11 @@
       <c r="E21" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -2285,8 +2353,11 @@
       <c r="E22" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -2299,8 +2370,11 @@
       <c r="D23" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -2313,8 +2387,11 @@
       <c r="D24" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -2327,8 +2404,11 @@
       <c r="D25" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>53</v>
       </c>
@@ -2341,8 +2421,11 @@
       <c r="D26" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -2355,8 +2438,11 @@
       <c r="D27" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
@@ -2369,8 +2455,11 @@
       <c r="D28" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>59</v>
       </c>
@@ -2383,8 +2472,11 @@
       <c r="D29" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>61</v>
       </c>
@@ -2397,8 +2489,11 @@
       <c r="D30" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>63</v>
       </c>
@@ -2411,8 +2506,11 @@
       <c r="D31" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>65</v>
       </c>
@@ -2428,8 +2526,11 @@
       <c r="E32" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>67</v>
       </c>
@@ -2442,8 +2543,11 @@
       <c r="D33" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>69</v>
       </c>
@@ -2456,8 +2560,11 @@
       <c r="D34" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>71</v>
       </c>
@@ -2470,8 +2577,11 @@
       <c r="D35" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>73</v>
       </c>
@@ -2484,8 +2594,11 @@
       <c r="D36" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>75</v>
       </c>
@@ -2498,8 +2611,11 @@
       <c r="D37" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>77</v>
       </c>
@@ -2512,8 +2628,11 @@
       <c r="D38" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>79</v>
       </c>
@@ -2526,8 +2645,11 @@
       <c r="D39" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>81</v>
       </c>
@@ -2540,8 +2662,11 @@
       <c r="D40" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>83</v>
       </c>
@@ -2554,8 +2679,11 @@
       <c r="D41" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>85</v>
       </c>
@@ -2568,8 +2696,11 @@
       <c r="D42" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>87</v>
       </c>
@@ -2585,8 +2716,11 @@
       <c r="E43" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>89</v>
       </c>
@@ -2599,8 +2733,11 @@
       <c r="D44" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>91</v>
       </c>
@@ -2613,8 +2750,11 @@
       <c r="D45" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>93</v>
       </c>
@@ -2627,8 +2767,11 @@
       <c r="D46" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>95</v>
       </c>
@@ -2641,8 +2784,11 @@
       <c r="D47" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>97</v>
       </c>
@@ -2655,8 +2801,11 @@
       <c r="D48" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>99</v>
       </c>
@@ -2669,8 +2818,11 @@
       <c r="D49" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>101</v>
       </c>
@@ -2683,8 +2835,11 @@
       <c r="D50" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>103</v>
       </c>
@@ -2697,8 +2852,11 @@
       <c r="D51" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>105</v>
       </c>
@@ -2711,8 +2869,11 @@
       <c r="D52" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>107</v>
       </c>
@@ -2725,8 +2886,11 @@
       <c r="D53" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>109</v>
       </c>
@@ -2739,8 +2903,11 @@
       <c r="D54" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>111</v>
       </c>
@@ -2753,8 +2920,11 @@
       <c r="D55" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>113</v>
       </c>
@@ -2767,8 +2937,11 @@
       <c r="D56" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>115</v>
       </c>
@@ -2781,8 +2954,11 @@
       <c r="D57" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>117</v>
       </c>
@@ -2795,8 +2971,11 @@
       <c r="D58" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>119</v>
       </c>
@@ -2812,8 +2991,11 @@
       <c r="E59" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>121</v>
       </c>
@@ -2829,8 +3011,11 @@
       <c r="E60" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>123</v>
       </c>
@@ -2846,8 +3031,11 @@
       <c r="E61" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>125</v>
       </c>
@@ -2860,8 +3048,11 @@
       <c r="D62" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>127</v>
       </c>
@@ -2877,8 +3068,11 @@
       <c r="E63" s="1" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>129</v>
       </c>
@@ -2894,8 +3088,11 @@
       <c r="E64" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>131</v>
       </c>
@@ -2908,8 +3105,11 @@
       <c r="D65" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>133</v>
       </c>
@@ -2925,8 +3125,11 @@
       <c r="E66" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>135</v>
       </c>
@@ -2942,8 +3145,11 @@
       <c r="E67" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>137</v>
       </c>
@@ -2959,8 +3165,11 @@
       <c r="E68" s="1" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>139</v>
       </c>
@@ -2976,8 +3185,11 @@
       <c r="E69" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>141</v>
       </c>
@@ -2993,8 +3205,11 @@
       <c r="E70" s="1" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>143</v>
       </c>
@@ -3010,8 +3225,11 @@
       <c r="E71" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>145</v>
       </c>
@@ -3027,8 +3245,11 @@
       <c r="E72" s="1" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>147</v>
       </c>
@@ -3044,8 +3265,11 @@
       <c r="E73" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" s="7" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>149</v>
       </c>
@@ -3058,8 +3282,11 @@
       <c r="D74" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>151</v>
       </c>
@@ -3072,8 +3299,11 @@
       <c r="D75" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>153</v>
       </c>
@@ -3086,8 +3316,11 @@
       <c r="D76" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>155</v>
       </c>
@@ -3100,8 +3333,11 @@
       <c r="D77" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>157</v>
       </c>
@@ -3114,8 +3350,11 @@
       <c r="D78" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>159</v>
       </c>
@@ -3128,8 +3367,11 @@
       <c r="D79" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>161</v>
       </c>
@@ -3142,8 +3384,11 @@
       <c r="D80" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F80" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>163</v>
       </c>
@@ -3156,8 +3401,11 @@
       <c r="D81" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F81" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>165</v>
       </c>
@@ -3170,8 +3418,11 @@
       <c r="D82" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F82" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>167</v>
       </c>
@@ -3184,8 +3435,11 @@
       <c r="D83" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F83" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>169</v>
       </c>
@@ -3198,8 +3452,11 @@
       <c r="D84" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F84" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>171</v>
       </c>
@@ -3212,8 +3469,11 @@
       <c r="D85" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F85" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>173</v>
       </c>
@@ -3226,8 +3486,11 @@
       <c r="D86" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F86" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>175</v>
       </c>
@@ -3240,8 +3503,11 @@
       <c r="D87" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F87" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>177</v>
       </c>
@@ -3254,8 +3520,11 @@
       <c r="D88" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F88" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>179</v>
       </c>
@@ -3268,8 +3537,11 @@
       <c r="D89" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F89" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>181</v>
       </c>
@@ -3282,8 +3554,11 @@
       <c r="D90" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F90" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>183</v>
       </c>
@@ -3296,8 +3571,11 @@
       <c r="D91" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F91" s="8" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>185</v>
       </c>
@@ -3310,8 +3588,11 @@
       <c r="D92" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F92" s="9" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>187</v>
       </c>
@@ -3324,8 +3605,11 @@
       <c r="D93" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F93" s="9" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>189</v>
       </c>
@@ -3338,8 +3622,11 @@
       <c r="D94" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F94" s="9" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>3</v>
       </c>
@@ -3352,8 +3639,11 @@
       <c r="D95" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F95" s="9" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>190</v>
       </c>
@@ -3366,8 +3656,11 @@
       <c r="D96" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F96" s="9" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>192</v>
       </c>
@@ -3379,6 +3672,9 @@
       </c>
       <c r="D97" t="s">
         <v>379</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -3390,7 +3686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6742B5D-D9C6-40F6-956B-8D4672EB2283}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>